<commit_message>
the add of the lastes changes
</commit_message>
<xml_diff>
--- a/Acceptance Testing/Expert-testing/Acceptance Testing.xlsx
+++ b/Acceptance Testing/Expert-testing/Acceptance Testing.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Variant 1" sheetId="2" r:id="rId1"/>
-    <sheet name="View referral details or result" sheetId="3" r:id="rId2"/>
+    <sheet name="verifying details" sheetId="3" r:id="rId2"/>
     <sheet name="view patient medical history" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="157">
   <si>
     <t xml:space="preserve">Use Case: </t>
   </si>
@@ -2319,25 +2319,6 @@
 Checking warning on an attempt to log in to a locked account.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Acceptance Testing for Use Case: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>View referral details or results</t>
-    </r>
-  </si>
-  <si>
-    <t>View referral details or results</t>
-  </si>
-  <si>
     <t>Export</t>
   </si>
   <si>
@@ -2363,40 +2344,6 @@
     </r>
   </si>
   <si>
-    <t>1. Expert enter the Patient ID
-2. if  Expert presses "show referral"
-3. SYSTEM System opens referral window
-4. if Expert presses "show results"
-5. SYSTEM System open result window</t>
-  </si>
-  <si>
-    <r>
-      <t>1.1 Expert enter Patient ID that doesn’t exsit in the System.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.2 System throws out a warning message and returns to main window.</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t>Scenario</t>
     </r>
@@ -2411,23 +2358,6 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve"> 5:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Scenario </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1:</t>
     </r>
   </si>
   <si>
@@ -3101,34 +3031,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>1.2.1 Expert enter a patient id , (for a patient that is not in his care) 
-1.2.2 Expert press on "show referral"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.2 System throws out a warning message,returns to main window  and clean the field.</t>
-    </r>
-  </si>
-  <si>
     <t>NoAccess</t>
   </si>
   <si>
@@ -3190,6 +3092,263 @@
       <t xml:space="preserve">
 Click "show referral detail" window. 
 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.2.1 Expert didn’t enter anything in patient id field 
+1.2.2 Expert press on "open"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.2 System throws out a warning message and returns to main window .</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.3.1 Expert enter a patient ID with one (or more) undigit chars.
+1.3.2 Expert press "open"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.3.3 System throws out a warning message, returns to main window and clean the field.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.2.1 Expert enter a patient id , (for a patient that is not in his care) 
+1.2.2 Expert press on "open"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.2 System throws out a warning message,returns to main window  and clean the field.</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Expert enters patients ID
+2. if patient ID not exist in DB
+3. SYSTEM show message "Id incorrect , please try again"
+4. Expert enters patient id correctly</t>
+  </si>
+  <si>
+    <t>Acceptance Testing for Use Case: verifying details</t>
+  </si>
+  <si>
+    <t>verifying details</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scenario </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.1 Expert enter Patient ID that doesn’t exsit in the System.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.2 System throws out a warning message and returns to main window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1.1:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.1.1 Expert enter a patient id , (for a patient that is not in his care) 
+1.1.2 Expert press on "show referral"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.1.3 System throws out a warning message,returns to main window  and clean the field.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4.1:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.1.1 Patient doesn't don’t have any details in the system (new Patient before the first appointment)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.1.2 System throws out a warning message and returns to main window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Open "verifying details" window.
+Type Patient ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3785234</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Click "ok" button. </t>
     </r>
   </si>
 </sst>
@@ -3365,7 +3524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -3904,11 +4063,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4073,6 +4245,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -4151,41 +4368,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4490,10 +4687,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="60"/>
+      <c r="C1" s="75"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -4557,10 +4754,10 @@
       <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="61" t="s">
+      <c r="C7" s="76" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="62"/>
+      <c r="D7" s="77"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" s="17"/>
@@ -4577,10 +4774,10 @@
       <c r="B9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="64"/>
+      <c r="D9" s="79"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
@@ -4589,10 +4786,10 @@
       <c r="B10" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="65" t="s">
+      <c r="C10" s="80" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="66"/>
+      <c r="D10" s="81"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
@@ -4601,10 +4798,10 @@
       <c r="B11" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="58" t="s">
+      <c r="C11" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="59"/>
+      <c r="D11" s="74"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
@@ -4613,10 +4810,10 @@
       <c r="B12" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="58" t="s">
+      <c r="C12" s="73" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="59"/>
+      <c r="D12" s="74"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
@@ -4625,10 +4822,10 @@
       <c r="B13" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="58" t="s">
+      <c r="C13" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="59"/>
+      <c r="D13" s="74"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -4637,10 +4834,10 @@
       <c r="B14" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="89" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="75"/>
+      <c r="D14" s="90"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
@@ -4720,11 +4917,11 @@
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="94" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="80"/>
-      <c r="D21" s="81"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="96"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
@@ -4821,10 +5018,10 @@
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="67">
+      <c r="A28" s="82">
         <v>4</v>
       </c>
-      <c r="B28" s="76" t="s">
+      <c r="B28" s="91" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -4833,35 +5030,35 @@
       <c r="D28" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="71" t="s">
+      <c r="E28" s="86" t="s">
         <v>80</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
-      <c r="B29" s="77"/>
+      <c r="A29" s="82"/>
+      <c r="B29" s="92"/>
       <c r="C29" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D29" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="72"/>
+      <c r="E29" s="87"/>
       <c r="F29" s="3"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="88.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="67"/>
-      <c r="B30" s="78"/>
+      <c r="A30" s="82"/>
+      <c r="B30" s="93"/>
       <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="73"/>
+      <c r="E30" s="88"/>
       <c r="F30" s="3"/>
       <c r="G30"/>
     </row>
@@ -4885,10 +5082,10 @@
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="67">
+      <c r="A32" s="82">
         <v>6</v>
       </c>
-      <c r="B32" s="68" t="s">
+      <c r="B32" s="83" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -4897,48 +5094,48 @@
       <c r="D32" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="71" t="s">
+      <c r="E32" s="86" t="s">
         <v>81</v>
       </c>
       <c r="F32"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="58.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="67"/>
-      <c r="B33" s="69"/>
+      <c r="A33" s="82"/>
+      <c r="B33" s="84"/>
       <c r="C33" s="48" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="72"/>
+      <c r="E33" s="87"/>
       <c r="F33"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="67"/>
-      <c r="B34" s="69"/>
+      <c r="A34" s="82"/>
+      <c r="B34" s="84"/>
       <c r="C34" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="72"/>
+      <c r="E34" s="87"/>
       <c r="F34"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="67"/>
-      <c r="B35" s="70"/>
+      <c r="A35" s="82"/>
+      <c r="B35" s="85"/>
       <c r="C35" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="73"/>
+      <c r="E35" s="88"/>
       <c r="F35"/>
       <c r="G35"/>
     </row>
@@ -5043,10 +5240,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5061,10 +5258,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" s="60"/>
+      <c r="B1" s="75" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="75"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -5083,7 +5280,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>85</v>
+        <v>149</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -5095,7 +5292,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
@@ -5107,7 +5304,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -5119,7 +5316,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -5130,13 +5327,11 @@
       <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="61" t="s">
-        <v>89</v>
-      </c>
-      <c r="D7" s="62"/>
+      <c r="C7" s="76" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="77"/>
       <c r="E7"/>
-      <c r="F7"/>
-      <c r="G7" s="17"/>
     </row>
     <row r="8" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="36"/>
@@ -5146,108 +5341,109 @@
       <c r="F8"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>139</v>
-      </c>
-      <c r="D9" s="64"/>
+        <v>152</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="79"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
     </row>
     <row r="10" spans="2:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="C10" s="63" t="s">
-        <v>140</v>
-      </c>
-      <c r="D10" s="64"/>
+        <v>136</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>135</v>
+      </c>
+      <c r="D10" s="79"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
     <row r="11" spans="2:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="33" t="s">
-        <v>142</v>
-      </c>
-      <c r="C11" s="63" t="s">
-        <v>144</v>
-      </c>
-      <c r="D11" s="64"/>
+        <v>137</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="79"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
-        <v>143</v>
-      </c>
-      <c r="C12" s="63" t="s">
-        <v>145</v>
-      </c>
-      <c r="D12" s="64"/>
-      <c r="E12"/>
-      <c r="F12"/>
-      <c r="G12"/>
-    </row>
-    <row r="13" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="33" t="s">
-        <v>112</v>
-      </c>
-      <c r="C13" s="63" t="s">
-        <v>113</v>
-      </c>
-      <c r="D13" s="64"/>
+        <v>150</v>
+      </c>
+      <c r="C12" s="78" t="s">
+        <v>151</v>
+      </c>
+      <c r="D12" s="79"/>
+    </row>
+    <row r="13" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="103" t="s">
+        <v>154</v>
+      </c>
+      <c r="C13" s="104" t="s">
+        <v>155</v>
+      </c>
+      <c r="D13" s="77"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="2:7" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="84" t="s">
-        <v>91</v>
-      </c>
-      <c r="C14" s="82" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="83"/>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="6"/>
+      <c r="C14"/>
+      <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
+    <row r="15" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="64" t="s">
+        <v>141</v>
+      </c>
       <c r="F16"/>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>95</v>
-      </c>
-      <c r="E17" s="90" t="s">
-        <v>147</v>
+      <c r="B17" s="25">
+        <v>3785234</v>
+      </c>
+      <c r="C17" s="4">
+        <v>467567</v>
+      </c>
+      <c r="D17" s="4">
+        <v>467567</v>
+      </c>
+      <c r="E17" s="67">
+        <v>1</v>
       </c>
       <c r="F17"/>
       <c r="G17"/>
@@ -5257,209 +5453,154 @@
         <v>3785234</v>
       </c>
       <c r="C18" s="4">
-        <v>467567</v>
+        <v>567523</v>
       </c>
       <c r="D18" s="4">
-        <v>467567</v>
-      </c>
-      <c r="E18" s="93">
-        <v>1</v>
+        <v>567523</v>
+      </c>
+      <c r="E18" s="67">
+        <v>2</v>
       </c>
       <c r="F18"/>
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B19" s="25">
-        <v>3785234</v>
-      </c>
-      <c r="C19" s="4">
-        <v>567523</v>
-      </c>
-      <c r="D19" s="4">
-        <v>567523</v>
-      </c>
-      <c r="E19" s="93">
+        <v>2222211</v>
+      </c>
+      <c r="C19" s="62">
+        <v>123358</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="68">
         <v>2</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="25">
-        <v>2222211</v>
-      </c>
-      <c r="C20" s="88">
-        <v>123358</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="94">
-        <v>2</v>
-      </c>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="60">
+        <v>4353476</v>
+      </c>
+      <c r="C20" s="61"/>
+      <c r="D20" s="61"/>
+      <c r="E20" s="69"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="86">
-        <v>4353476</v>
-      </c>
-      <c r="C21" s="87"/>
-      <c r="D21" s="87"/>
-      <c r="E21" s="95"/>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
       <c r="F21"/>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22"/>
-      <c r="F22"/>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="52" t="s">
+    </row>
+    <row r="22" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>15</v>
+      </c>
       <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>15</v>
-      </c>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" ht="44.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="53">
+        <v>1</v>
+      </c>
+      <c r="B24" s="56" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>156</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>92</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="3"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53">
-        <v>1</v>
-      </c>
-      <c r="B25" s="56" t="s">
-        <v>96</v>
-      </c>
-      <c r="C25" s="54" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="54" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="10"/>
+        <v>4</v>
+      </c>
+      <c r="B25" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>127</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="53">
-        <v>2</v>
-      </c>
-      <c r="B26" s="56" t="s">
-        <v>98</v>
-      </c>
-      <c r="C26" s="54" t="s">
-        <v>100</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>101</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>105</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="12"/>
       <c r="F26" s="3"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="53">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>102</v>
+        <v>140</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>103</v>
+        <v>143</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>106</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E27" s="12"/>
       <c r="F27" s="3"/>
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53">
-        <v>4</v>
-      </c>
-      <c r="B28" s="27" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>137</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>134</v>
-      </c>
-      <c r="E28" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28"/>
-    </row>
-    <row r="29" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="53">
-        <v>5</v>
-      </c>
-      <c r="B29" s="27" t="s">
-        <v>133</v>
-      </c>
-      <c r="C29" s="9" t="s">
-        <v>135</v>
-      </c>
-      <c r="D29" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="E29" s="12"/>
-      <c r="F29" s="3"/>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="53">
-        <v>6</v>
-      </c>
-      <c r="B30" s="27" t="s">
-        <v>146</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="E30" s="12"/>
-      <c r="F30" s="3"/>
-      <c r="G30"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C12:D12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5468,10 +5609,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5486,10 +5627,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="60" t="s">
-        <v>107</v>
-      </c>
-      <c r="C1" s="60"/>
+      <c r="B1" s="75" t="s">
+        <v>102</v>
+      </c>
+      <c r="C1" s="75"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -5508,7 +5649,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -5520,7 +5661,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4"/>
       <c r="E4"/>
@@ -5532,7 +5673,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -5544,7 +5685,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -5555,10 +5696,10 @@
       <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="61" t="s">
-        <v>111</v>
-      </c>
-      <c r="D7" s="62"/>
+      <c r="C7" s="76" t="s">
+        <v>106</v>
+      </c>
+      <c r="D7" s="77"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" s="17"/>
@@ -5571,421 +5712,701 @@
       <c r="F8"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="2:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
-        <v>92</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" s="64"/>
+        <v>133</v>
+      </c>
+      <c r="C9" s="78" t="s">
+        <v>134</v>
+      </c>
+      <c r="D9" s="79"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="84" t="s">
-        <v>88</v>
-      </c>
-      <c r="C10" s="82" t="s">
-        <v>114</v>
-      </c>
-      <c r="D10" s="83"/>
+    <row r="10" spans="2:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>144</v>
+      </c>
+      <c r="D10" s="79"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
-      <c r="C11"/>
-      <c r="D11"/>
+    <row r="11" spans="2:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="78" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="79"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12"/>
-      <c r="D12"/>
+    <row r="12" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="33" t="s">
+        <v>138</v>
+      </c>
+      <c r="C12" s="78" t="s">
+        <v>146</v>
+      </c>
+      <c r="D12" s="79"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B13" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="D13" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="E13" s="89" t="s">
-        <v>117</v>
-      </c>
-      <c r="F13" s="90" t="s">
-        <v>118</v>
-      </c>
+    <row r="13" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="D13" s="98"/>
+      <c r="E13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B14" s="25">
-        <v>3785234</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E14" s="4">
-        <v>20</v>
-      </c>
-      <c r="F14" s="85" t="s">
-        <v>118</v>
-      </c>
+    <row r="14" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="33" t="s">
+        <v>107</v>
+      </c>
+      <c r="C14" s="78" t="s">
+        <v>108</v>
+      </c>
+      <c r="D14" s="79"/>
+      <c r="E14"/>
       <c r="G14"/>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B15" s="25">
-        <v>2345236</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E15" s="4">
-        <v>16</v>
-      </c>
-      <c r="F15" s="85" t="s">
-        <v>118</v>
-      </c>
+    <row r="15" spans="2:7" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="97" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="98"/>
+      <c r="E15"/>
       <c r="G15"/>
     </row>
-    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="86">
-        <v>2222211</v>
-      </c>
-      <c r="C16" s="87" t="s">
-        <v>123</v>
-      </c>
-      <c r="D16" s="87" t="s">
-        <v>124</v>
-      </c>
-      <c r="E16" s="91">
-        <v>50</v>
-      </c>
-      <c r="F16" s="92" t="s">
-        <v>118</v>
-      </c>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B16" s="6"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
       <c r="G16"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="C17"/>
       <c r="D17"/>
       <c r="E17"/>
-      <c r="F17"/>
-    </row>
-    <row r="18" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="52" t="s">
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B18" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D18" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="E18" s="63" t="s">
+        <v>112</v>
+      </c>
+      <c r="F18" s="63" t="s">
+        <v>141</v>
+      </c>
+      <c r="G18" s="64" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="25">
+        <v>3785234</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="4">
+        <v>20</v>
+      </c>
+      <c r="F19" s="62">
+        <v>1</v>
+      </c>
+      <c r="G19" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="25">
+        <v>2345236</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" s="4">
+        <v>16</v>
+      </c>
+      <c r="F20" s="62">
+        <v>2</v>
+      </c>
+      <c r="G20" s="59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="60">
+        <v>2222211</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>118</v>
+      </c>
+      <c r="D21" s="61" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="65">
+        <v>50</v>
+      </c>
+      <c r="F21" s="102">
+        <v>2</v>
+      </c>
+      <c r="G21" s="66" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22" s="99"/>
+      <c r="F22" s="100"/>
+      <c r="G22" s="101"/>
+    </row>
+    <row r="23" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="52"/>
-      <c r="D18" s="52"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
+      <c r="C23" s="52"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B24" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="29" t="s">
+      <c r="C24" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="D19" s="29" t="s">
+      <c r="D24" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E24" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F19" s="3"/>
-      <c r="G19"/>
-    </row>
-    <row r="20" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="53">
-        <v>1</v>
-      </c>
-      <c r="B20" s="56" t="s">
-        <v>125</v>
-      </c>
-      <c r="C20" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="D20" s="54" t="s">
-        <v>127</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20"/>
-    </row>
-    <row r="21" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="53">
-        <v>2</v>
-      </c>
-      <c r="B21" s="56" t="s">
-        <v>129</v>
-      </c>
-      <c r="C21" s="54" t="s">
-        <v>126</v>
-      </c>
-      <c r="D21" s="54" t="s">
-        <v>130</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>78</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21"/>
-    </row>
-    <row r="22" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="53">
-        <v>3</v>
-      </c>
-      <c r="B22" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" s="3"/>
-      <c r="G22"/>
-    </row>
-    <row r="23" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A23" s="67">
-        <v>4</v>
-      </c>
-      <c r="B23" s="76" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E23" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="3"/>
-      <c r="G23"/>
-    </row>
-    <row r="24" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A24" s="67"/>
-      <c r="B24" s="77"/>
-      <c r="C24" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="D24" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="E24" s="72"/>
       <c r="F24" s="3"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" ht="88.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="67"/>
-      <c r="B25" s="78"/>
-      <c r="C25" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D25" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E25" s="73"/>
+    <row r="25" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="53">
+        <v>1</v>
+      </c>
+      <c r="B25" s="56" t="s">
+        <v>120</v>
+      </c>
+      <c r="C25" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="D25" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>123</v>
+      </c>
       <c r="F25" s="3"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>5</v>
-      </c>
-      <c r="B26" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D26" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>24</v>
+      <c r="A26" s="53">
+        <v>2</v>
+      </c>
+      <c r="B26" s="56" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="D26" s="54" t="s">
+        <v>125</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>78</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A27" s="67">
+    <row r="27" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="53">
+        <v>3</v>
+      </c>
+      <c r="B27" s="56" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="54" t="s">
+        <v>48</v>
+      </c>
+      <c r="D27" s="54" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="F27" s="3"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
+      <c r="A28" s="82">
+        <v>4</v>
+      </c>
+      <c r="B28" s="91" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="F28" s="3"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.2">
+      <c r="A29" s="82"/>
+      <c r="B29" s="92"/>
+      <c r="C29" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>71</v>
+      </c>
+      <c r="E29" s="87"/>
+      <c r="F29" s="3"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7" ht="88.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="82"/>
+      <c r="B30" s="93"/>
+      <c r="C30" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D30" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="E30" s="88"/>
+      <c r="F30" s="3"/>
+      <c r="G30"/>
+    </row>
+    <row r="31" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>5</v>
+      </c>
+      <c r="B31" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" s="42" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="3"/>
+      <c r="G31"/>
+    </row>
+    <row r="32" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
+      <c r="A32" s="82">
         <v>6</v>
       </c>
-      <c r="B27" s="68" t="s">
+      <c r="B32" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C32" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="14" t="s">
+      <c r="D32" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E27" s="71" t="s">
+      <c r="E32" s="86" t="s">
         <v>81</v>
       </c>
-      <c r="F27"/>
-      <c r="G27"/>
-    </row>
-    <row r="28" spans="1:7" ht="58.5" x14ac:dyDescent="0.2">
-      <c r="A28" s="67"/>
-      <c r="B28" s="69"/>
-      <c r="C28" s="55" t="s">
+      <c r="F32"/>
+      <c r="G32"/>
+    </row>
+    <row r="33" spans="1:7" ht="58.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="82"/>
+      <c r="B33" s="84"/>
+      <c r="C33" s="55" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="55" t="s">
+      <c r="D33" s="55" t="s">
         <v>25</v>
       </c>
-      <c r="E28" s="72"/>
-      <c r="F28"/>
-      <c r="G28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" s="67"/>
-      <c r="B29" s="69"/>
-      <c r="C29" s="18" t="s">
+      <c r="E33" s="87"/>
+      <c r="F33"/>
+      <c r="G33"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="82"/>
+      <c r="B34" s="84"/>
+      <c r="C34" s="18" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="19" t="s">
+      <c r="D34" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E29" s="72"/>
-      <c r="F29"/>
-      <c r="G29"/>
-    </row>
-    <row r="30" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="67"/>
-      <c r="B30" s="70"/>
-      <c r="C30" s="16" t="s">
+      <c r="E34" s="87"/>
+      <c r="F34"/>
+      <c r="G34"/>
+    </row>
+    <row r="35" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="82"/>
+      <c r="B35" s="85"/>
+      <c r="C35" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="D30" s="21" t="s">
+      <c r="D35" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E30" s="73"/>
-      <c r="F30"/>
-      <c r="G30"/>
-    </row>
-    <row r="31" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="53">
+      <c r="E35" s="88"/>
+      <c r="F35"/>
+      <c r="G35"/>
+    </row>
+    <row r="36" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="53">
         <v>7</v>
       </c>
-      <c r="B31" s="31" t="s">
+      <c r="B36" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C36" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D31" s="57" t="s">
+      <c r="D36" s="57" t="s">
         <v>52</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E36" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="F31"/>
-      <c r="G31"/>
-    </row>
-    <row r="32" spans="1:7" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="53">
+      <c r="F36"/>
+      <c r="G36"/>
+    </row>
+    <row r="37" spans="1:7" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="53">
         <v>8</v>
       </c>
-      <c r="B32" s="31" t="s">
+      <c r="B37" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="9" t="s">
+      <c r="C37" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="D32" s="57" t="s">
+      <c r="D37" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="E32" s="9" t="s">
+      <c r="E37" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="F32" s="3"/>
-      <c r="G32"/>
-    </row>
-    <row r="33" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="53">
+      <c r="F37" s="3"/>
+      <c r="G37"/>
+    </row>
+    <row r="38" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="53">
         <v>9</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B38" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="9" t="s">
+      <c r="C38" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="57" t="s">
+      <c r="D38" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E38" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F33" s="3"/>
-      <c r="G33"/>
-    </row>
-    <row r="34" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="F38" s="3"/>
+      <c r="G38"/>
+    </row>
+    <row r="39" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
         <v>10</v>
       </c>
-      <c r="B34" s="51" t="s">
+      <c r="B39" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="9" t="s">
+      <c r="C39" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="D39" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E39" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="F34" s="3"/>
-      <c r="G34"/>
+      <c r="F39" s="3"/>
+      <c r="G39"/>
+    </row>
+    <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C59"/>
+      <c r="D59"/>
+      <c r="E59"/>
+      <c r="F59"/>
+      <c r="G59"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B60" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C60" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="D60" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F60"/>
+      <c r="G60"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B61" s="25">
+        <v>3785234</v>
+      </c>
+      <c r="C61" s="4">
+        <v>467567</v>
+      </c>
+      <c r="D61" s="4">
+        <v>467567</v>
+      </c>
+      <c r="F61"/>
+      <c r="G61"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B62" s="25">
+        <v>3785234</v>
+      </c>
+      <c r="C62" s="4">
+        <v>567523</v>
+      </c>
+      <c r="D62" s="4">
+        <v>567523</v>
+      </c>
+      <c r="F62"/>
+      <c r="G62"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B63" s="25">
+        <v>2222211</v>
+      </c>
+      <c r="C63" s="62">
+        <v>123358</v>
+      </c>
+      <c r="D63" s="4"/>
+      <c r="F63"/>
+      <c r="G63"/>
+    </row>
+    <row r="64" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="60">
+        <v>4353476</v>
+      </c>
+      <c r="C64" s="61"/>
+      <c r="D64" s="61"/>
+      <c r="F64"/>
+      <c r="G64"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C65"/>
+      <c r="D65"/>
+      <c r="E65"/>
+      <c r="F65"/>
+    </row>
+    <row r="66" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="52"/>
+      <c r="D66" s="52"/>
+      <c r="E66" s="52"/>
+      <c r="F66" s="3"/>
+    </row>
+    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D67" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F67" s="3"/>
+      <c r="G67"/>
+    </row>
+    <row r="68" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="70">
+        <v>1</v>
+      </c>
+      <c r="B68" s="72" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="71" t="s">
+        <v>94</v>
+      </c>
+      <c r="D68" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="E68" s="10"/>
+      <c r="F68" s="3"/>
+      <c r="G68"/>
+    </row>
+    <row r="69" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="70">
+        <v>2</v>
+      </c>
+      <c r="B69" s="72" t="s">
+        <v>93</v>
+      </c>
+      <c r="C69" s="71" t="s">
+        <v>95</v>
+      </c>
+      <c r="D69" s="71" t="s">
+        <v>96</v>
+      </c>
+      <c r="E69" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F69" s="3"/>
+      <c r="G69"/>
+    </row>
+    <row r="70" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="70">
+        <v>3</v>
+      </c>
+      <c r="B70" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D70" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E70" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="F70" s="3"/>
+      <c r="G70"/>
+    </row>
+    <row r="71" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="70">
+        <v>4</v>
+      </c>
+      <c r="B71" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="D71" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="E71" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="F71" s="3"/>
+      <c r="G71"/>
+    </row>
+    <row r="72" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="70">
+        <v>5</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>128</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="D72" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="E72" s="12"/>
+      <c r="F72" s="3"/>
+      <c r="G72"/>
+    </row>
+    <row r="73" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="70">
+        <v>6</v>
+      </c>
+      <c r="B73" s="27" t="s">
+        <v>140</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="D73" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E73" s="12"/>
+      <c r="F73" s="3"/>
+      <c r="G73"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="B27:B30"/>
-    <mergeCell ref="E27:E30"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="E23:E25"/>
+  <mergeCells count="15">
+    <mergeCell ref="E32:E35"/>
+    <mergeCell ref="A28:A30"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="E28:E30"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C13:D13"/>
     <mergeCell ref="C9:D9"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="B32:B35"/>
     <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update to the testing
</commit_message>
<xml_diff>
--- a/Acceptance Testing/Expert-testing/Acceptance Testing.xlsx
+++ b/Acceptance Testing/Expert-testing/Acceptance Testing.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11415" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11415" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Variant 1" sheetId="2" r:id="rId1"/>
     <sheet name="verifying details" sheetId="3" r:id="rId2"/>
-    <sheet name="view patient medical history" sheetId="4" r:id="rId3"/>
+    <sheet name="Record appointment" sheetId="4" r:id="rId3"/>
+    <sheet name="Produce referral for lab test" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="162">
   <si>
     <t xml:space="preserve">Use Case: </t>
   </si>
@@ -2327,44 +2328,6 @@
 patient has a medical records file</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Scenario </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scenario</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 5:</t>
-    </r>
-  </si>
-  <si>
-    <t>5.1 Patient doesn't don’t have any referral result in the system (new Patient).
-5.2 System throws out a warning message and returns to main window.</t>
-  </si>
-  <si>
     <t>referral details (serial number)</t>
   </si>
   <si>
@@ -2401,7 +2364,47 @@
     </r>
   </si>
   <si>
-    <t>NoReferralDetailsFound</t>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>…</t>
+  </si>
+  <si>
+    <t>Blankentering</t>
+  </si>
+  <si>
+    <t>the Expert enter an ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UnDigitsValuesEnter </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A system throws out a warning 
+message </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"you didn’t enter any patient ID, please enter one".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The system clean the Patient ID Field.</t>
+    </r>
   </si>
   <si>
     <r>
@@ -2417,7 +2420,29 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>3785234</t>
+      <t>378</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>234</t>
     </r>
     <r>
       <rPr>
@@ -2436,19 +2461,46 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">A system throws out a warning 
+message </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">"you have enter an undigit char to the Patient ID field, please Re-enter the ID".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The system clean the Patient ID Field.</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t>Open "view referral details or result" window.
 Type Patient ID:</t>
     </r>
     <r>
       <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>4353476</t>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>___</t>
     </r>
     <r>
       <rPr>
@@ -2465,6 +2517,102 @@
   </si>
   <si>
     <r>
+      <t>1.2.1 Expert didn’t enter anything in patient id field 
+1.2.2 Expert press on "show referral"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.2 System throws out a warning message and returns to main window .</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scenario </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.2:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1.3:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.3.1 Expert enter a patient ID with one (or more) undigit chars.
+1.3.2 Expert press "show referral"</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.3.3 System throws out a warning message, returns to main window and clean the field.</t>
+    </r>
+  </si>
+  <si>
+    <t>NoAccess</t>
+  </si>
+  <si>
+    <t>Expert in care</t>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">A system throws out a warning 
 message </t>
     </r>
@@ -2477,7 +2625,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>"Patient 4353476 do not have any referral"</t>
+      <t>"Patient 3785234 his not under your care, Access Denied"</t>
     </r>
     <r>
       <rPr>
@@ -2492,11 +2640,9 @@
     </r>
   </si>
   <si>
-    <t>NoReferralResultsFound</t>
-  </si>
-  <si>
-    <r>
-      <t>Open "view referral details or result" window.
+    <r>
+      <t>Expert for heart-problems do a login (as 2)
+Open "view referral details or result" window.
 Type Patient ID:</t>
     </r>
     <r>
@@ -2508,363 +2654,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>2222211</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Click "show referral detail" window. 
-Open "show referral detail" window.
-Clik "show referral result" window.
-Open "show referral result" window.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A system throws out a warning 
-message </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Patient 2222211 do not have any referral Result".</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">
-The patient doesn’t have any referral.</t>
-  </si>
-  <si>
-    <t>The patient doesn’t have any referral Result.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Acceptance Testing for Use Case: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFC00000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>view patient medical history</t>
-    </r>
-  </si>
-  <si>
-    <t>view patient medical history</t>
-  </si>
-  <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>LoginExpert has logged in and was identified as expert
-patient has a medical records file</t>
-  </si>
-  <si>
-    <t>1. Expert enter the Patient ID
-2. Expert presses "open" on patients medical record file
-3.  Expert presses "view History"
-4. SYSTEM System searches patients  medical record file
-5. if medical record file is found
-6. SYSTEM  System shows medical record on screen
-7. else 
-8. SYSTEM  System alerts with "no medical record has been found"</t>
-  </si>
-  <si>
-    <r>
-      <t>Scenario</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 3.1:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>3.1.1 Patient doesn't don’t have any details in the system (new Patient before the first appointment)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3.1.2 System throws out a warning message and returns to main window.</t>
-    </r>
-  </si>
-  <si>
-    <t>4.1 System search for patient recored 
-4.2 After 5 min the system throw out a warning message
-4.3 System return to "view patient medical history window"</t>
-  </si>
-  <si>
-    <t>First name</t>
-  </si>
-  <si>
-    <t>Last name</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>…</t>
-  </si>
-  <si>
-    <t>Yossi</t>
-  </si>
-  <si>
-    <t>chone</t>
-  </si>
-  <si>
-    <t>Rotem</t>
-  </si>
-  <si>
-    <t>levi</t>
-  </si>
-  <si>
-    <t>Ziv</t>
-  </si>
-  <si>
-    <t>Palty</t>
-  </si>
-  <si>
-    <t>SuccessfulResult</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Open "view patient medical history"
-type Patient ID: </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
       <t>3785234</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-click on patients medical record file
-</t>
-    </r>
-  </si>
-  <si>
-    <t>Expert get acsess to patient 3785234 medical recored.</t>
-  </si>
-  <si>
-    <t>watch only, no change</t>
-  </si>
-  <si>
-    <t>NoMedicalRecored</t>
-  </si>
-  <si>
-    <r>
-      <t>A system throws out a warning 
-message "</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>the system don’t have any medical info</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">".
-</t>
-    </r>
-  </si>
-  <si>
-    <t>Blankentering</t>
-  </si>
-  <si>
-    <t>the Expert enter an ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UnDigitsValuesEnter </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A system throws out a warning 
-message </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"you didn’t enter any patient ID, please enter one".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The system clean the Patient ID Field.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Open "view referral details or result" window.
-Type Patient ID:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>378</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>s</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>234</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Click "show referral detail" window. 
-Open "show referral detail" window.
-Clik "show referral result" window.
-Open "show referral result" window.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A system throws out a warning 
-message </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">"you have enter an undigit char to the Patient ID field, please Re-enter the ID".
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>The system clean the Patient ID Field.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Open "view referral details or result" window.
-Type Patient ID:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>___</t>
     </r>
     <r>
       <rPr>
@@ -2880,6 +2670,12 @@
     </r>
   </si>
   <si>
+    <t>Acceptance Testing for Use Case: verifying details</t>
+  </si>
+  <si>
+    <t>verifying details</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Scenario </t>
     </r>
@@ -2893,12 +2689,57 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.1:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.1.1 Expert enter Patient ID that doesn’t exsit in the System.</t>
+      <t>2:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2.1 Expert enter Patient ID that doesn’t exsit in the System.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.2 System throws out a warning message and returns to main window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 1.1:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1.1.1 Expert enter a patient id , (for a patient that is not in his care) 
+1.1.2 Expert press on "show referral"</t>
     </r>
     <r>
       <rPr>
@@ -2920,13 +2761,133 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.1.2 System throws out a warning message and returns to main window.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.2.1 Expert didn’t enter anything in patient id field 
-1.2.2 Expert press on "show referral"</t>
+      <t>1.1.3 System throws out a warning message,returns to main window  and clean the field.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Scenario</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 4.1:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4.1.1 Patient doesn't don’t have any details in the system (new Patient before the first appointment)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.1.2 System throws out a warning message and returns to main window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Open "verifying details" window.
+Type Patient ID:</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3785234</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Click "ok" button. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Acceptance Testing for Use Case: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Record appointment</t>
+    </r>
+  </si>
+  <si>
+    <t>Record appointment</t>
+  </si>
+  <si>
+    <t>LoginExpert has logged in and was identified as expert
+patient has to have a apointment to this doctor</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">2.1 Expert press on "record" button
+2.2 System throws out a warning message "Another doctor his already recording on this document, doctor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>____</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" and return to verifiying details.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">3.1.1 Expert press in "record" but do not write anything </t>
     </r>
     <r>
       <rPr>
@@ -2948,7 +2909,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.2 System throws out a warning message and returns to main window .</t>
+      <t>3.1.2 System throws out a warning message and returns to Record appointment window .</t>
     </r>
   </si>
   <si>
@@ -2965,12 +2926,12 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>1.2:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scenario</t>
+      <t>3.1:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Scenario </t>
     </r>
     <r>
       <rPr>
@@ -2982,238 +2943,283 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 1.3:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scenario</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
+      <t>7:</t>
+    </r>
+  </si>
+  <si>
+    <t>7.1 System try to save record but do not Successd  
+7.2 System throw out a warning message "unable to save the record, please try again" and return to "Record appointment" window.</t>
+  </si>
+  <si>
+    <t>apointment Record</t>
+  </si>
+  <si>
+    <t>…..</t>
+  </si>
+  <si>
+    <t>Date of the appointment</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expert press on "record" button 
+Expert record the appointment in medical file 
+Expert press save
+SYSTEM display "report sent successfully"
+</t>
+  </si>
+  <si>
+    <t>SuccessApointmentRecord</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expert Succeed to Record the appointment </t>
+  </si>
+  <si>
+    <t>UמArrivePaintent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expert press on "record" button 
+Expert report that the patient didn't come
+Expert press save
+SYSTEM display "report sent successfully"
+</t>
+  </si>
+  <si>
+    <t>Expert Succeed to Record the the paintent didn’t Arrive</t>
+  </si>
+  <si>
+    <t>EmptyRecording</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expert press on "record" button 
+Expert record the appointment in medical file 
+Expert press save
+</t>
+  </si>
+  <si>
+    <r>
+      <t>A system throws out a warning 
+message "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>you did not enter any info in to your appointment recording</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>".
+Return to the "Record appointment" window.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">
+Checking mandatory fields.
+The recording field is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFC00000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>empty</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Checking mandatory fields.
+The recording field is not empty</t>
+  </si>
+  <si>
+    <t>MultiRecordingError</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Expert press on "record" button 
+</t>
+  </si>
+  <si>
+    <r>
+      <t>A system throws out a warning 
+message "</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Another doctor his already recording on this document, doctor </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> 1.4:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.3.1 Expert enter a patient ID with one (or more) undigit chars.
-1.3.2 Expert press "show referral"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.3.3 System throws out a warning message, returns to main window and clean the field.</t>
-    </r>
-  </si>
-  <si>
-    <t>NoAccess</t>
-  </si>
-  <si>
-    <t>Expert in care</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A system throws out a warning 
-message </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Patient 3785234 his not under your care, Access Denied"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-A system clean the Patient ID fields.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Expert for heart-problems do a login (as 2)
-Open "view referral details or result" window.
-Type Patient ID:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3785234</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Click "show referral detail" window. 
-</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.2.1 Expert didn’t enter anything in patient id field 
-1.2.2 Expert press on "open"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.2 System throws out a warning message and returns to main window .</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.3.1 Expert enter a patient ID with one (or more) undigit chars.
-1.3.2 Expert press "open"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.3.3 System throws out a warning message, returns to main window and clean the field.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.2.1 Expert enter a patient id , (for a patient that is not in his care) 
-1.2.2 Expert press on "open"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.2 System throws out a warning message,returns to main window  and clean the field.</t>
-    </r>
+      <t>____</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>".
+Return to the "Record appointment" window.</t>
+    </r>
+  </si>
+  <si>
+    <t>file open in doctor account</t>
+  </si>
+  <si>
+    <t>cheak if the Account id is not open in other doctor account</t>
+  </si>
+  <si>
+    <t>0 - not open in any doctor account</t>
+  </si>
+  <si>
+    <t>(not 0) - doctor user account</t>
+  </si>
+  <si>
+    <t>patient ID</t>
+  </si>
+  <si>
+    <t>LoginExpert has logged in and was identified as expert</t>
+  </si>
+  <si>
+    <t>lab worker</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Acceptance Testing for Use Case: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Produce referral for lab test</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Expert chooses type of referral
+2. Expert files notes for lab worker
+3. if Expert presses "Produce referral"
+   4. SYSTEM forward referral to lab worker
+   5. SYSTEM display message " referral sent"
+6. else if Expert presses on button "cancel"
+   7. SYSTEM System cleans all fields
+   8. SYSTEM System returns to patients medical file</t>
+  </si>
+  <si>
+    <t>1. include: patient not arrived to appointment
+2. Expert press on "record" button 
+3. if Patient didn't arrive
+   4. Expert report that the patient didn't come
+5. else 
+   6.Expert record the appointment in medical file 
+   7. SYSTEM display "report sent successfully"</t>
   </si>
   <si>
     <t>1. Expert enters patients ID
 2. if patient ID not exist in DB
-3. SYSTEM show message "Id incorrect , please try again"
-4. Expert enters patient id correctly</t>
-  </si>
-  <si>
-    <t>Acceptance Testing for Use Case: verifying details</t>
-  </si>
-  <si>
-    <t>verifying details</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Scenario </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>2:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>2.1 Expert enter Patient ID that doesn’t exsit in the System.</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+  3. SYSTEM show message "Id incorrect , please try again"
+  4. Expert enters patient id correctly</t>
+  </si>
+  <si>
+    <t>Scenario 3.1:</t>
+  </si>
+  <si>
+    <t>3.1.1 Expert didn’t fill the type_of_referral
+3.1.2 System throws out a warning message and returns to Prodouce referral for lab text window.</t>
+  </si>
+  <si>
+    <t>type of referral</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Blood Test</t>
+  </si>
+  <si>
+    <t>ECG</t>
+  </si>
+  <si>
+    <t>SuccessfulProduce</t>
+  </si>
+  <si>
+    <r>
+      <t>SYSTEM display message " referral sent"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">expert fill the form  
+System forward referral to lab worker
+</t>
+  </si>
+  <si>
+    <r>
+      <t>Expert chooses type of referral :</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> blood test</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
@@ -3221,44 +3227,21 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
-2</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.2 System throws out a warning message and returns to main window.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scenario</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 1.1:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>1.1.1 Expert enter a patient id , (for a patient that is not in his care) 
-1.1.2 Expert press on "show referral"</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
+Expert files notes for lab worker: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>blood type A+</t>
+    </r>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Arial"/>
@@ -3266,89 +3249,8 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">
+Expert press "send"
 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>1.1.3 System throws out a warning message,returns to main window  and clean the field.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Scenario</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> 4.1:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>4.1.1 Patient doesn't don’t have any details in the system (new Patient before the first appointment)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.
-4</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.1.2 System throws out a warning message and returns to main window.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Open "verifying details" window.
-Type Patient ID:</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>3785234</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Click "ok" button. </t>
     </r>
   </si>
 </sst>
@@ -3486,7 +3388,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3523,6 +3425,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="43">
     <border>
@@ -4080,7 +3988,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="118">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4236,51 +4144,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4289,84 +4188,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
@@ -4375,14 +4196,140 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4671,8 +4618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4687,10 +4634,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="91" t="s">
         <v>36</v>
       </c>
-      <c r="C1" s="75"/>
+      <c r="C1" s="91"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -4754,10 +4701,10 @@
       <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="76" t="s">
+      <c r="C7" s="92" t="s">
         <v>54</v>
       </c>
-      <c r="D7" s="77"/>
+      <c r="D7" s="93"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" s="17"/>
@@ -4774,10 +4721,10 @@
       <c r="B9" s="33" t="s">
         <v>50</v>
       </c>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="94" t="s">
         <v>53</v>
       </c>
-      <c r="D9" s="79"/>
+      <c r="D9" s="95"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
@@ -4786,10 +4733,10 @@
       <c r="B10" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="80" t="s">
+      <c r="C10" s="96" t="s">
         <v>76</v>
       </c>
-      <c r="D10" s="81"/>
+      <c r="D10" s="97"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
@@ -4798,10 +4745,10 @@
       <c r="B11" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="81" t="s">
         <v>65</v>
       </c>
-      <c r="D11" s="74"/>
+      <c r="D11" s="82"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
@@ -4810,10 +4757,10 @@
       <c r="B12" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="73" t="s">
+      <c r="C12" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="74"/>
+      <c r="D12" s="82"/>
       <c r="E12"/>
       <c r="F12"/>
       <c r="G12"/>
@@ -4822,10 +4769,10 @@
       <c r="B13" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="73" t="s">
+      <c r="C13" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="D13" s="74"/>
+      <c r="D13" s="82"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -4834,10 +4781,10 @@
       <c r="B14" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C14" s="89" t="s">
+      <c r="C14" s="83" t="s">
         <v>64</v>
       </c>
-      <c r="D14" s="90"/>
+      <c r="D14" s="84"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
@@ -4917,11 +4864,11 @@
       <c r="G20"/>
     </row>
     <row r="21" spans="1:7" ht="43.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="94" t="s">
+      <c r="B21" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="C21" s="95"/>
-      <c r="D21" s="96"/>
+      <c r="C21" s="89"/>
+      <c r="D21" s="90"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
@@ -5018,10 +4965,10 @@
       <c r="G27"/>
     </row>
     <row r="28" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="82">
+      <c r="A28" s="74">
         <v>4</v>
       </c>
-      <c r="B28" s="91" t="s">
+      <c r="B28" s="85" t="s">
         <v>21</v>
       </c>
       <c r="C28" s="13" t="s">
@@ -5030,35 +4977,35 @@
       <c r="D28" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="86" t="s">
+      <c r="E28" s="78" t="s">
         <v>80</v>
       </c>
       <c r="F28" s="3"/>
       <c r="G28"/>
     </row>
     <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A29" s="82"/>
-      <c r="B29" s="92"/>
+      <c r="A29" s="74"/>
+      <c r="B29" s="86"/>
       <c r="C29" s="48" t="s">
         <v>70</v>
       </c>
       <c r="D29" s="48" t="s">
         <v>71</v>
       </c>
-      <c r="E29" s="87"/>
+      <c r="E29" s="79"/>
       <c r="F29" s="3"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="88.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="82"/>
-      <c r="B30" s="93"/>
+      <c r="A30" s="74"/>
+      <c r="B30" s="87"/>
       <c r="C30" s="15" t="s">
         <v>35</v>
       </c>
       <c r="D30" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="E30" s="88"/>
+      <c r="E30" s="80"/>
       <c r="F30" s="3"/>
       <c r="G30"/>
     </row>
@@ -5082,10 +5029,10 @@
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="82">
+      <c r="A32" s="74">
         <v>6</v>
       </c>
-      <c r="B32" s="83" t="s">
+      <c r="B32" s="75" t="s">
         <v>29</v>
       </c>
       <c r="C32" s="13" t="s">
@@ -5094,48 +5041,48 @@
       <c r="D32" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="86" t="s">
+      <c r="E32" s="78" t="s">
         <v>81</v>
       </c>
       <c r="F32"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="58.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
-      <c r="B33" s="84"/>
+      <c r="A33" s="74"/>
+      <c r="B33" s="76"/>
       <c r="C33" s="48" t="s">
         <v>30</v>
       </c>
       <c r="D33" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="87"/>
+      <c r="E33" s="79"/>
       <c r="F33"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="82"/>
-      <c r="B34" s="84"/>
+      <c r="A34" s="74"/>
+      <c r="B34" s="76"/>
       <c r="C34" s="18" t="s">
         <v>74</v>
       </c>
       <c r="D34" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="E34" s="87"/>
+      <c r="E34" s="79"/>
       <c r="F34"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
-      <c r="B35" s="85"/>
+      <c r="A35" s="74"/>
+      <c r="B35" s="77"/>
       <c r="C35" s="16" t="s">
         <v>51</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E35" s="88"/>
+      <c r="E35" s="80"/>
       <c r="F35"/>
       <c r="G35"/>
     </row>
@@ -5217,6 +5164,12 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="A32:A35"/>
     <mergeCell ref="B32:B35"/>
     <mergeCell ref="E32:E35"/>
@@ -5226,12 +5179,6 @@
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="E28:E30"/>
     <mergeCell ref="B21:D21"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" verticalDpi="0" r:id="rId1"/>
@@ -5242,8 +5189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5258,10 +5205,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="75" t="s">
-        <v>148</v>
-      </c>
-      <c r="C1" s="75"/>
+      <c r="B1" s="91" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="91"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -5280,7 +5227,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -5304,7 +5251,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -5327,10 +5274,10 @@
       <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="76" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" s="77"/>
+      <c r="C7" s="92" t="s">
+        <v>151</v>
+      </c>
+      <c r="D7" s="93"/>
       <c r="E7"/>
     </row>
     <row r="8" spans="2:7" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -5343,57 +5290,57 @@
     </row>
     <row r="9" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
-        <v>152</v>
-      </c>
-      <c r="C9" s="78" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="79"/>
+        <v>111</v>
+      </c>
+      <c r="C9" s="94" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="95"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
     </row>
     <row r="10" spans="2:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B10" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="78" t="s">
-        <v>135</v>
-      </c>
-      <c r="D10" s="79"/>
+        <v>100</v>
+      </c>
+      <c r="C10" s="94" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="95"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
     <row r="11" spans="2:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="78" t="s">
-        <v>139</v>
-      </c>
-      <c r="D11" s="79"/>
+        <v>101</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11" s="95"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
     </row>
     <row r="12" spans="2:7" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="33" t="s">
-        <v>150</v>
-      </c>
-      <c r="C12" s="78" t="s">
-        <v>151</v>
-      </c>
-      <c r="D12" s="79"/>
+        <v>109</v>
+      </c>
+      <c r="C12" s="94" t="s">
+        <v>110</v>
+      </c>
+      <c r="D12" s="95"/>
     </row>
     <row r="13" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="103" t="s">
-        <v>154</v>
-      </c>
-      <c r="C13" s="104" t="s">
-        <v>155</v>
-      </c>
-      <c r="D13" s="77"/>
+      <c r="B13" s="73" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="98" t="s">
+        <v>114</v>
+      </c>
+      <c r="D13" s="93"/>
       <c r="E13"/>
       <c r="F13"/>
       <c r="G13"/>
@@ -5421,13 +5368,13 @@
         <v>8</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>90</v>
-      </c>
-      <c r="E16" s="64" t="s">
-        <v>141</v>
+        <v>87</v>
+      </c>
+      <c r="E16" s="61" t="s">
+        <v>104</v>
       </c>
       <c r="F16"/>
       <c r="G16"/>
@@ -5442,7 +5389,7 @@
       <c r="D17" s="4">
         <v>467567</v>
       </c>
-      <c r="E17" s="67">
+      <c r="E17" s="63">
         <v>1</v>
       </c>
       <c r="F17"/>
@@ -5458,7 +5405,7 @@
       <c r="D18" s="4">
         <v>567523</v>
       </c>
-      <c r="E18" s="67">
+      <c r="E18" s="63">
         <v>2</v>
       </c>
       <c r="F18"/>
@@ -5468,23 +5415,23 @@
       <c r="B19" s="25">
         <v>2222211</v>
       </c>
-      <c r="C19" s="62">
+      <c r="C19" s="60">
         <v>123358</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="68">
+      <c r="E19" s="64">
         <v>2</v>
       </c>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="60">
+      <c r="B20" s="58">
         <v>4353476</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="69"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="65"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -5526,14 +5473,14 @@
       <c r="A24" s="53">
         <v>1</v>
       </c>
-      <c r="B24" s="56" t="s">
-        <v>91</v>
+      <c r="B24" s="55" t="s">
+        <v>88</v>
       </c>
       <c r="C24" s="54" t="s">
-        <v>156</v>
+        <v>115</v>
       </c>
       <c r="D24" s="54" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="E24" s="10"/>
       <c r="F24" s="3"/>
@@ -5544,16 +5491,16 @@
         <v>4</v>
       </c>
       <c r="B25" s="27" t="s">
-        <v>126</v>
+        <v>92</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>129</v>
+        <v>95</v>
       </c>
       <c r="E25" s="12" t="s">
-        <v>127</v>
+        <v>93</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25"/>
@@ -5563,13 +5510,13 @@
         <v>5</v>
       </c>
       <c r="B26" s="27" t="s">
-        <v>128</v>
+        <v>94</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="E26" s="12"/>
       <c r="F26" s="3"/>
@@ -5580,13 +5527,13 @@
         <v>6</v>
       </c>
       <c r="B27" s="27" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
       <c r="E27" s="12"/>
       <c r="F27" s="3"/>
@@ -5609,16 +5556,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G73"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="2.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="45.5" style="5" customWidth="1"/>
     <col min="4" max="4" width="37.875" style="5" customWidth="1"/>
     <col min="5" max="5" width="24.375" style="5" bestFit="1" customWidth="1"/>
@@ -5627,10 +5574,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B1" s="75" t="s">
-        <v>102</v>
-      </c>
-      <c r="C1" s="75"/>
+      <c r="B1" s="91" t="s">
+        <v>116</v>
+      </c>
+      <c r="C1" s="91"/>
       <c r="D1"/>
       <c r="E1"/>
       <c r="F1"/>
@@ -5649,7 +5596,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="D3"/>
       <c r="E3"/>
@@ -5673,7 +5620,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="32" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="D5"/>
       <c r="E5"/>
@@ -5685,7 +5632,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="D6"/>
       <c r="E6"/>
@@ -5696,10 +5643,10 @@
       <c r="B7" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="76" t="s">
-        <v>106</v>
-      </c>
-      <c r="D7" s="77"/>
+      <c r="C7" s="92" t="s">
+        <v>150</v>
+      </c>
+      <c r="D7" s="93"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" s="17"/>
@@ -5712,701 +5659,843 @@
       <c r="F8"/>
       <c r="G8"/>
     </row>
-    <row r="9" spans="2:7" ht="28.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:7" ht="49.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="33" t="s">
-        <v>133</v>
-      </c>
-      <c r="C9" s="78" t="s">
-        <v>134</v>
-      </c>
-      <c r="D9" s="79"/>
+        <v>109</v>
+      </c>
+      <c r="C9" s="94" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="95"/>
       <c r="E9"/>
       <c r="F9"/>
       <c r="G9"/>
     </row>
-    <row r="10" spans="2:7" ht="48.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:7" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="33" t="s">
-        <v>136</v>
-      </c>
-      <c r="C10" s="78" t="s">
-        <v>144</v>
-      </c>
-      <c r="D10" s="79"/>
+        <v>121</v>
+      </c>
+      <c r="C10" s="94" t="s">
+        <v>120</v>
+      </c>
+      <c r="D10" s="95"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="2:7" ht="46.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="33" t="s">
-        <v>137</v>
-      </c>
-      <c r="C11" s="78" t="s">
-        <v>145</v>
-      </c>
-      <c r="D11" s="79"/>
+    <row r="11" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="56" t="s">
+        <v>122</v>
+      </c>
+      <c r="C11" s="99" t="s">
+        <v>123</v>
+      </c>
+      <c r="D11" s="100"/>
       <c r="E11"/>
-      <c r="F11"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="2:7" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="33" t="s">
-        <v>138</v>
-      </c>
-      <c r="C12" s="78" t="s">
-        <v>146</v>
-      </c>
-      <c r="D12" s="79"/>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="6"/>
+      <c r="C12"/>
+      <c r="D12"/>
       <c r="E12"/>
-      <c r="F12"/>
       <c r="G12"/>
     </row>
-    <row r="13" spans="2:7" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="58" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="97" t="s">
-        <v>109</v>
-      </c>
-      <c r="D13" s="98"/>
+    <row r="13" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
       <c r="E13"/>
       <c r="G13"/>
     </row>
-    <row r="14" spans="2:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="33" t="s">
-        <v>107</v>
-      </c>
-      <c r="C14" s="78" t="s">
-        <v>108</v>
-      </c>
-      <c r="D14" s="79"/>
-      <c r="E14"/>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>86</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="E14" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="F14" s="61" t="s">
+        <v>141</v>
+      </c>
       <c r="G14"/>
     </row>
-    <row r="15" spans="2:7" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="58" t="s">
-        <v>87</v>
-      </c>
-      <c r="C15" s="97" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" s="98"/>
-      <c r="E15"/>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="25">
+        <v>3785234</v>
+      </c>
+      <c r="C15" s="109">
+        <v>342342</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E15" s="101">
+        <v>42873</v>
+      </c>
+      <c r="F15" s="57">
+        <v>1</v>
+      </c>
       <c r="G15"/>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B16" s="6"/>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
+      <c r="B16" s="25">
+        <v>2345236</v>
+      </c>
+      <c r="C16" s="109">
+        <v>234234</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="101">
+        <v>42590</v>
+      </c>
+      <c r="F16" s="57">
+        <v>2</v>
+      </c>
       <c r="G16"/>
     </row>
     <row r="17" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C17"/>
-      <c r="D17"/>
-      <c r="E17"/>
+      <c r="B17" s="58">
+        <v>2222211</v>
+      </c>
+      <c r="C17" s="110">
+        <v>123574</v>
+      </c>
+      <c r="D17" s="59" t="s">
+        <v>125</v>
+      </c>
+      <c r="E17" s="102">
+        <v>42070</v>
+      </c>
+      <c r="F17" s="62">
+        <v>0</v>
+      </c>
       <c r="G17"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="D18" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="E18" s="63" t="s">
-        <v>112</v>
-      </c>
-      <c r="F18" s="63" t="s">
+      <c r="B18" s="108" t="s">
         <v>141</v>
       </c>
-      <c r="G18" s="64" t="s">
-        <v>113</v>
-      </c>
+      <c r="C18" s="106" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="107" t="s">
+        <v>144</v>
+      </c>
+      <c r="E18" s="106"/>
+      <c r="F18"/>
+      <c r="G18"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="25">
-        <v>3785234</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="E19" s="4">
-        <v>20</v>
-      </c>
-      <c r="F19" s="62">
+      <c r="B19" s="103"/>
+      <c r="C19" s="104"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="72"/>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20" s="70"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="72"/>
+    </row>
+    <row r="21" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F22" s="3"/>
+      <c r="G22"/>
+    </row>
+    <row r="23" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="53">
         <v>1</v>
       </c>
-      <c r="G19" s="59" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="25">
-        <v>2345236</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="E20" s="4">
-        <v>16</v>
-      </c>
-      <c r="F20" s="62">
+      <c r="B23" s="69" t="s">
+        <v>128</v>
+      </c>
+      <c r="C23" s="68" t="s">
+        <v>127</v>
+      </c>
+      <c r="D23" s="68" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F23" s="3"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="53">
         <v>2</v>
       </c>
-      <c r="G20" s="59" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="60">
-        <v>2222211</v>
-      </c>
-      <c r="C21" s="61" t="s">
-        <v>118</v>
-      </c>
-      <c r="D21" s="61" t="s">
-        <v>119</v>
-      </c>
-      <c r="E21" s="65">
-        <v>50</v>
-      </c>
-      <c r="F21" s="102">
-        <v>2</v>
-      </c>
-      <c r="G21" s="66" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C22"/>
-      <c r="D22"/>
-      <c r="E22" s="99"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="101"/>
-    </row>
-    <row r="23" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="52"/>
-      <c r="D23" s="52"/>
-      <c r="E23" s="52"/>
-      <c r="F23" s="3"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D24" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E24" s="30" t="s">
-        <v>15</v>
-      </c>
+      <c r="B24" s="69" t="s">
+        <v>130</v>
+      </c>
+      <c r="C24" s="68" t="s">
+        <v>131</v>
+      </c>
+      <c r="D24" s="68" t="s">
+        <v>132</v>
+      </c>
+      <c r="E24" s="10"/>
       <c r="F24" s="3"/>
       <c r="G24"/>
     </row>
-    <row r="25" spans="1:7" ht="58.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="53">
-        <v>1</v>
-      </c>
-      <c r="B25" s="56" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="D25" s="54" t="s">
-        <v>122</v>
+        <v>3</v>
+      </c>
+      <c r="B25" s="69" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="68" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="68" t="s">
+        <v>135</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="F25" s="3"/>
       <c r="G25"/>
     </row>
-    <row r="26" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="53">
-        <v>2</v>
-      </c>
-      <c r="B26" s="56" t="s">
-        <v>124</v>
-      </c>
-      <c r="C26" s="54" t="s">
-        <v>121</v>
-      </c>
-      <c r="D26" s="54" t="s">
-        <v>125</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>78</v>
+    <row r="26" spans="1:7" ht="74.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>5</v>
+      </c>
+      <c r="B26" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>142</v>
       </c>
       <c r="F26" s="3"/>
       <c r="G26"/>
     </row>
-    <row r="27" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53">
-        <v>3</v>
-      </c>
-      <c r="B27" s="56" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="54" t="s">
-        <v>48</v>
-      </c>
-      <c r="D27" s="54" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F27" s="3"/>
+    <row r="27" spans="1:7" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G27"/>
     </row>
-    <row r="28" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A28" s="82">
-        <v>4</v>
-      </c>
-      <c r="B28" s="91" t="s">
-        <v>21</v>
-      </c>
-      <c r="C28" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="86" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="3"/>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G28"/>
     </row>
-    <row r="29" spans="1:7" ht="45" x14ac:dyDescent="0.2">
-      <c r="A29" s="82"/>
-      <c r="B29" s="92"/>
-      <c r="C29" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="D29" s="55" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="87"/>
-      <c r="F29" s="3"/>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G29"/>
     </row>
-    <row r="30" spans="1:7" ht="88.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="82"/>
-      <c r="B30" s="93"/>
-      <c r="C30" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D30" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="E30" s="88"/>
-      <c r="F30" s="3"/>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G30"/>
     </row>
-    <row r="31" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>5</v>
-      </c>
-      <c r="B31" s="27" t="s">
-        <v>22</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D31" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F31" s="3"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G31"/>
     </row>
-    <row r="32" spans="1:7" ht="59.25" x14ac:dyDescent="0.2">
-      <c r="A32" s="82">
-        <v>6</v>
-      </c>
-      <c r="B32" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="C32" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D32" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="86" t="s">
-        <v>81</v>
-      </c>
-      <c r="F32"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G32"/>
     </row>
-    <row r="33" spans="1:7" ht="58.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="82"/>
-      <c r="B33" s="84"/>
-      <c r="C33" s="55" t="s">
-        <v>30</v>
-      </c>
-      <c r="D33" s="55" t="s">
-        <v>25</v>
-      </c>
-      <c r="E33" s="87"/>
-      <c r="F33"/>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" s="82"/>
-      <c r="B34" s="84"/>
-      <c r="C34" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="D34" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="E34" s="87"/>
-      <c r="F34"/>
       <c r="G34"/>
     </row>
-    <row r="35" spans="1:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
-      <c r="B35" s="85"/>
-      <c r="C35" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="D35" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E35" s="88"/>
-      <c r="F35"/>
-      <c r="G35"/>
-    </row>
-    <row r="36" spans="1:7" ht="72" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="53">
-        <v>7</v>
-      </c>
-      <c r="B36" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="D36" s="57" t="s">
-        <v>52</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="F36"/>
-      <c r="G36"/>
-    </row>
-    <row r="37" spans="1:7" ht="86.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="53">
-        <v>8</v>
-      </c>
-      <c r="B37" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="F37" s="3"/>
-      <c r="G37"/>
-    </row>
-    <row r="38" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="53">
-        <v>9</v>
-      </c>
-      <c r="B38" s="27" t="s">
-        <v>41</v>
-      </c>
-      <c r="C38" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D38" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="E38" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="F38" s="3"/>
-      <c r="G38"/>
-    </row>
-    <row r="39" spans="1:7" ht="60" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>10</v>
-      </c>
-      <c r="B39" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="D39" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="E39" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="F39" s="3"/>
-      <c r="G39"/>
-    </row>
-    <row r="59" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="7" t="s">
-        <v>6</v>
-      </c>
+    <row r="42" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A42" s="3"/>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+    </row>
+    <row r="43" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+    </row>
+    <row r="44" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+    </row>
+    <row r="46" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="3"/>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+    </row>
+    <row r="47" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A47" s="3"/>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+    </row>
+    <row r="48" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="3"/>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+    </row>
+    <row r="49" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+    </row>
+    <row r="50" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+    </row>
+    <row r="51" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+    </row>
+    <row r="52" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A52" s="3"/>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+    </row>
+    <row r="53" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A53" s="3"/>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+    </row>
+    <row r="54" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A54"/>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+    </row>
+    <row r="55" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A55"/>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+    </row>
+    <row r="56" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A56"/>
+      <c r="B56"/>
+      <c r="C56"/>
+      <c r="D56"/>
+      <c r="E56"/>
+      <c r="F56"/>
+      <c r="G56"/>
+    </row>
+    <row r="57" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A57"/>
+      <c r="B57"/>
+      <c r="C57"/>
+      <c r="D57"/>
+      <c r="E57"/>
+      <c r="F57"/>
+      <c r="G57"/>
+    </row>
+    <row r="58" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A58"/>
+      <c r="B58"/>
+      <c r="C58"/>
+      <c r="D58"/>
+      <c r="E58"/>
+      <c r="F58"/>
+      <c r="G58"/>
+    </row>
+    <row r="59" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A59"/>
+      <c r="B59"/>
       <c r="C59"/>
       <c r="D59"/>
       <c r="E59"/>
       <c r="F59"/>
       <c r="G59"/>
     </row>
-    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B60" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C60" s="23" t="s">
-        <v>89</v>
-      </c>
-      <c r="D60" s="23" t="s">
-        <v>90</v>
-      </c>
+    <row r="60" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A60" s="3"/>
+      <c r="B60"/>
+      <c r="C60"/>
+      <c r="D60"/>
+      <c r="E60"/>
       <c r="F60"/>
       <c r="G60"/>
     </row>
-    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B61" s="25">
-        <v>3785234</v>
-      </c>
-      <c r="C61" s="4">
-        <v>467567</v>
-      </c>
-      <c r="D61" s="4">
-        <v>467567</v>
-      </c>
+    <row r="61" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A61" s="3"/>
+      <c r="B61"/>
+      <c r="C61"/>
+      <c r="D61"/>
+      <c r="E61"/>
       <c r="F61"/>
       <c r="G61"/>
     </row>
-    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B62" s="25">
-        <v>3785234</v>
-      </c>
-      <c r="C62" s="4">
-        <v>567523</v>
-      </c>
-      <c r="D62" s="4">
-        <v>567523</v>
-      </c>
+    <row r="62" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A62"/>
+      <c r="B62"/>
+      <c r="C62"/>
+      <c r="D62"/>
+      <c r="E62"/>
       <c r="F62"/>
       <c r="G62"/>
     </row>
-    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B63" s="25">
-        <v>2222211</v>
-      </c>
-      <c r="C63" s="62">
-        <v>123358</v>
-      </c>
-      <c r="D63" s="4"/>
+    <row r="63" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A63"/>
+      <c r="B63"/>
+      <c r="C63"/>
+      <c r="D63"/>
+      <c r="E63"/>
       <c r="F63"/>
       <c r="G63"/>
     </row>
-    <row r="64" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B64" s="60">
-        <v>4353476</v>
-      </c>
-      <c r="C64" s="61"/>
-      <c r="D64" s="61"/>
+    <row r="64" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
+      <c r="A64"/>
+      <c r="B64"/>
+      <c r="C64"/>
+      <c r="D64"/>
+      <c r="E64"/>
       <c r="F64"/>
       <c r="G64"/>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="C65"/>
-      <c r="D65"/>
-      <c r="E65"/>
-      <c r="F65"/>
-    </row>
-    <row r="66" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B66" s="52" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="52"/>
-      <c r="D66" s="52"/>
-      <c r="E66" s="52"/>
-      <c r="F66" s="3"/>
-    </row>
-    <row r="67" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B67" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="D67" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="E67" s="30" t="s">
-        <v>15</v>
-      </c>
-      <c r="F67" s="3"/>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G65"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.2">
+      <c r="G66"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G67"/>
     </row>
-    <row r="68" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="70">
-        <v>1</v>
-      </c>
-      <c r="B68" s="72" t="s">
-        <v>91</v>
-      </c>
-      <c r="C68" s="71" t="s">
-        <v>94</v>
-      </c>
-      <c r="D68" s="71" t="s">
-        <v>92</v>
-      </c>
-      <c r="E68" s="10"/>
-      <c r="F68" s="3"/>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.2">
       <c r="G68"/>
     </row>
-    <row r="69" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="70">
-        <v>2</v>
-      </c>
-      <c r="B69" s="72" t="s">
-        <v>93</v>
-      </c>
-      <c r="C69" s="71" t="s">
-        <v>95</v>
-      </c>
-      <c r="D69" s="71" t="s">
-        <v>96</v>
-      </c>
-      <c r="E69" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="F69" s="3"/>
-      <c r="G69"/>
-    </row>
-    <row r="70" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="70">
-        <v>3</v>
-      </c>
-      <c r="B70" s="27" t="s">
-        <v>97</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="E70" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F70" s="3"/>
-      <c r="G70"/>
-    </row>
-    <row r="71" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="70">
-        <v>4</v>
-      </c>
-      <c r="B71" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="E71" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" s="3"/>
-      <c r="G71"/>
-    </row>
-    <row r="72" spans="1:7" ht="87" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="70">
-        <v>5</v>
-      </c>
-      <c r="B72" s="27" t="s">
-        <v>128</v>
-      </c>
-      <c r="C72" s="9" t="s">
-        <v>130</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>131</v>
-      </c>
-      <c r="E72" s="12"/>
-      <c r="F72" s="3"/>
-      <c r="G72"/>
-    </row>
-    <row r="73" spans="1:7" ht="59.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="70">
-        <v>6</v>
-      </c>
-      <c r="B73" s="27" t="s">
-        <v>140</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="E73" s="12"/>
-      <c r="F73" s="3"/>
-      <c r="G73"/>
-    </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="E32:E35"/>
-    <mergeCell ref="A28:A30"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="E28:E30"/>
+  <mergeCells count="5">
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C11:D11"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="B32:B35"/>
     <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C15:D15"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="2.75" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.5" style="5" customWidth="1"/>
+    <col min="4" max="4" width="37.875" style="5" customWidth="1"/>
+    <col min="5" max="5" width="24.375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5" style="5" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="3" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="91" t="s">
+        <v>148</v>
+      </c>
+      <c r="C1" s="91"/>
+      <c r="D1"/>
+      <c r="E1"/>
+      <c r="F1"/>
+      <c r="G1"/>
+    </row>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B2" s="5"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>147</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+    </row>
+    <row r="6" spans="2:7" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+    </row>
+    <row r="7" spans="2:7" ht="126" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="92" t="s">
+        <v>149</v>
+      </c>
+      <c r="D7" s="93"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7" s="17"/>
+    </row>
+    <row r="8" spans="2:7" ht="7.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="36"/>
+      <c r="C8" s="37"/>
+      <c r="D8" s="38"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+    </row>
+    <row r="9" spans="2:7" ht="35.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="112" t="s">
+        <v>152</v>
+      </c>
+      <c r="C9" s="113" t="s">
+        <v>153</v>
+      </c>
+      <c r="D9" s="114"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+    </row>
+    <row r="10" spans="2:7" ht="40.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="56"/>
+      <c r="C10" s="115"/>
+      <c r="D10" s="116"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+    </row>
+    <row r="11" spans="2:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="6"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+    </row>
+    <row r="12" spans="2:7" ht="31.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+    </row>
+    <row r="13" spans="2:7" ht="28.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>154</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B14" s="25">
+        <v>3785234</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="25">
+        <v>2345236</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="58">
+        <v>2222211</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>156</v>
+      </c>
+      <c r="D16" s="111" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+    </row>
+    <row r="18" spans="1:7" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18"/>
+      <c r="G18"/>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="30" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
+    <row r="20" spans="1:7" ht="54.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="67">
+        <v>1</v>
+      </c>
+      <c r="B20" s="69" t="s">
+        <v>158</v>
+      </c>
+      <c r="C20" s="117" t="s">
+        <v>161</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>159</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F20"/>
+      <c r="G20"/>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="67"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="10"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="67"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="68"/>
+      <c r="D22" s="68"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="67"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="66"/>
+      <c r="E23" s="9"/>
+      <c r="F23"/>
+      <c r="G23"/>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="67"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="66"/>
+      <c r="E24" s="9"/>
+      <c r="F24"/>
+      <c r="G24"/>
+    </row>
+    <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="67"/>
+      <c r="B25" s="27"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="66"/>
+      <c r="E25" s="20"/>
+      <c r="F25"/>
+      <c r="G25"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="51"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="20"/>
+      <c r="F26"/>
+      <c r="G26"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F27"/>
+      <c r="G27"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F28" s="3"/>
+      <c r="G28"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F29" s="3"/>
+      <c r="G29"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="F30" s="3"/>
+      <c r="G30"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>